<commit_message>
problem definition added, update bom
</commit_message>
<xml_diff>
--- a/stage-1-documents/CSE321-project3-terckerts-bom.xlsx
+++ b/stage-1-documents/CSE321-project3-terckerts-bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26914747c5e4c1a5/Documents/senior-year/CSE-321/cse321-project-3/stage-1-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C7D7C0C-9D99-446E-9B03-40CC595BC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{2C7D7C0C-9D99-446E-9B03-40CC595BC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98F44687-0C51-4EE6-86B7-1BC17FF7AE56}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{34829551-FD21-44A2-9BE5-92BE2B1DA078}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Timothy Erckert</t>
   </si>
@@ -90,14 +90,55 @@
   </si>
   <si>
     <t>Gikfun Metal Ball Tilt Shaking Position Switches</t>
+  </si>
+  <si>
+    <t>Male-to-male jumper wires</t>
+  </si>
+  <si>
+    <t>Female-to-male jumper wires</t>
+  </si>
+  <si>
+    <t>Microcontroller board, controls the program</t>
+  </si>
+  <si>
+    <t>Used to display menus and options to a user</t>
+  </si>
+  <si>
+    <t>Control current flow to LEDs</t>
+  </si>
+  <si>
+    <t>Allows user to interact with menu options</t>
+  </si>
+  <si>
+    <t>Prototyping board, used to design board layout</t>
+  </si>
+  <si>
+    <t>Detects when board is uneven</t>
+  </si>
+  <si>
+    <t>Provides audio feedback to user</t>
+  </si>
+  <si>
+    <t>Provide visual feedback to user</t>
+  </si>
+  <si>
+    <t>Connects components</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,17 +162,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -148,6 +230,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,15 +535,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72990A33-66B5-4E4A-8267-3241793A68E4}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -470,145 +556,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="12">
         <v>1602</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="C8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="4" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>